<commit_message>
updated URLs and prices
</commit_message>
<xml_diff>
--- a/platoon/logistics/plattonPartsList.xlsx
+++ b/platoon/logistics/plattonPartsList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>Raspberry Pi</t>
   </si>
@@ -24,12 +24,6 @@
     <t>Model</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>512 MB RAM</t>
-  </si>
-  <si>
     <t>OS</t>
   </si>
   <si>
@@ -57,18 +51,9 @@
     <t>Maxbotix LV-EZ1</t>
   </si>
   <si>
-    <t>N-Channel power MOSFET</t>
-  </si>
-  <si>
     <t>LED Breadboard connection</t>
   </si>
   <si>
-    <t>AC-DC CONV, EXTERNAL PLUG IN, 1A, MICRO-USB</t>
-  </si>
-  <si>
-    <t>Breadboard</t>
-  </si>
-  <si>
     <t>TIP 120 Power Transistor</t>
   </si>
   <si>
@@ -84,18 +69,12 @@
     <t>M2</t>
   </si>
   <si>
-    <t>Power LCD</t>
-  </si>
-  <si>
     <t>Purchase from</t>
   </si>
   <si>
     <t>Element14.com</t>
   </si>
   <si>
-    <t>Pi plate</t>
-  </si>
-  <si>
     <t xml:space="preserve">PCB for RaspberryPi </t>
   </si>
   <si>
@@ -117,9 +96,6 @@
     <t>Basic 16x2 Character LCD White on Black 5V</t>
   </si>
   <si>
-    <t>Power Supply for Rpi</t>
-  </si>
-  <si>
     <t>12V for Arduino.  Will power LEDs also</t>
   </si>
   <si>
@@ -138,9 +114,6 @@
     <t xml:space="preserve">EDIMAX  Wireless Nano Adapter  </t>
   </si>
   <si>
-    <t>802.11b/g/n USB 2.0 Up to 150Mbps</t>
-  </si>
-  <si>
     <t>newegg.com</t>
   </si>
   <si>
@@ -169,6 +142,66 @@
   </si>
   <si>
     <t>Arduino Power supply</t>
+  </si>
+  <si>
+    <t>http://www.newegg.com/Product/Product.aspx?Item=N82E16812117321</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/jsp/search/productdetail.jsp?SKU=43W5302&amp;CMP=KNC-GPLA</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/adafruit-industries/801/prototyping-pi-plate-kit-raspberry/dp/44W3453?in_merch=Popular%20Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coboc USB-6-AB-W 6 ft. USB 2.0 A Male to B Male Cable M-M - OEM </t>
+  </si>
+  <si>
+    <t>Power Supply for Raspberry Pi, AC-DC CONV, EXTERNAL PLUG IN, 1A, MICRO-USB</t>
+  </si>
+  <si>
+    <t>Rpi to Arduino comms</t>
+  </si>
+  <si>
+    <t>LCD and Range Sensor management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED, OSC Server, Webserver, remote administration of Rpi and Arduino </t>
+  </si>
+  <si>
+    <t>44W3453</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Prototyping Pi Plate Kit</t>
+  </si>
+  <si>
+    <t>N82E16812117321</t>
+  </si>
+  <si>
+    <t>Newegg.com</t>
+  </si>
+  <si>
+    <t>newark.com</t>
+  </si>
+  <si>
+    <t>newark</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/arduino/a000077/daughter-card-arduino-proto-shield/dp/78T1602?in_merch=Popular%20Products&amp;MER=PPSO_N_C_EverywhereElse_None</t>
+  </si>
+  <si>
+    <t>Arduino Protoplate</t>
+  </si>
+  <si>
+    <t>Arduino circuit connections</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/TIP120/TIP120-ND/1052441?adpos=1t2&amp;WT.term=tip120&amp;WT.mc_id=Fairchild+Semiconductor&amp;WT.medium=cpc&amp;WT.campaign=Fairchild+Semiconductor&amp;WT.content=text&amp;WT.srch=1&amp;type=Phrase&amp;WT.source=google&amp;cshift_ck=C7AE7C92-6598-4FF3-8753-DFB42457ACE3csbKXepAwP&amp;network=g</t>
+  </si>
+  <si>
+    <t>http://www.newegg.com/Product/Product.aspx?Item=N82E16833315091</t>
   </si>
 </sst>
 </file>
@@ -178,7 +211,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,8 +234,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,8 +270,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -245,11 +300,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -257,7 +335,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -269,8 +346,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,519 +679,526 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J2:J3"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="119.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="J1" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
+      <c r="B2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="17" t="s">
+        <v>49</v>
+      </c>
       <c r="G2" s="4">
         <v>1</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>35</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <f>G2*H2</f>
         <v>35</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>24</v>
+      <c r="J2" s="12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
-        <v>26</v>
+      <c r="A3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="4">
+        <v>801</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>15.95</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <f>G3*H3</f>
         <v>15.95</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="J3" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="25">
+        <v>1</v>
+      </c>
+      <c r="H4" s="27">
         <v>6.95</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="27">
         <f>G4*H4</f>
         <v>6.95</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>24</v>
+      <c r="J4" s="25" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="A5" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="25">
+        <v>1</v>
+      </c>
+      <c r="H5" s="27">
         <v>4.95</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="27">
         <f>G5*H5</f>
         <v>4.95</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25">
+        <v>22</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="25">
+        <v>1</v>
+      </c>
+      <c r="H6" s="27">
+        <v>25.19</v>
+      </c>
+      <c r="I6" s="27">
+        <f t="shared" ref="I6:I17" si="0">G6*H6</f>
+        <v>25.19</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="25">
+        <v>1</v>
+      </c>
+      <c r="H7" s="27">
+        <v>13.33</v>
+      </c>
+      <c r="I7" s="27">
+        <f t="shared" si="0"/>
+        <v>13.33</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4">
-        <v>22</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-      <c r="H6" s="6">
-        <v>25.19</v>
-      </c>
-      <c r="I6" s="6">
-        <f t="shared" ref="I6:I13" si="0">G6*H6</f>
-        <v>25.19</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="F7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="4">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6">
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
         <v>25.95</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I9" s="5">
         <f t="shared" si="0"/>
         <v>25.95</v>
       </c>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6">
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
         <v>9.9499999999999993</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I10" s="5">
         <f t="shared" si="0"/>
         <v>9.9499999999999993</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="4">
-        <v>3</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="4"/>
+      <c r="J10" s="12" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>16</v>
+      <c r="A11" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="G11" s="4">
-        <v>1</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10">
+        <v>3</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0.51</v>
+      </c>
+      <c r="I11" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="4"/>
+        <v>1.53</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>32</v>
+      <c r="A12" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>31</v>
+      <c r="F12" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="G12" s="4">
         <v>1</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>15.95</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <f t="shared" si="0"/>
         <v>15.95</v>
       </c>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>28</v>
+      <c r="A13" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
-        <v>30</v>
+      <c r="F13" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="G13" s="4">
         <v>1</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>0.95</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>18</v>
+      <c r="A14" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
-        <v>20</v>
+      <c r="F14" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="G14" s="4">
         <v>6</v>
       </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4">
-        <v>1</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="4"/>
+      <c r="A15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="14">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4">
-        <v>1</v>
-      </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>37</v>
+      <c r="A16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="14">
+        <v>1</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="4"/>
+      <c r="F17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1</v>
+      </c>
+      <c r="H17" s="15">
+        <v>1.22</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" si="0"/>
+        <v>1.22</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="8"/>
+      <c r="A18" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="4"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="9">
-        <f>SUM(I2:I10)</f>
-        <v>123.94000000000001</v>
-      </c>
-      <c r="J18" s="4"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8">
+        <f>SUM(I2:I17)</f>
+        <v>156.91999999999999</v>
+      </c>
+      <c r="J19" s="19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22">
-        <v>22</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22">
-        <v>5</v>
-      </c>
-      <c r="H22" s="1">
-        <v>29.95</v>
-      </c>
-      <c r="I22" s="1">
-        <f t="shared" ref="I22:I23" si="1">G22*H22</f>
-        <v>149.75</v>
-      </c>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="F23" s="2"/>
-      <c r="G23">
-        <v>18</v>
-      </c>
-      <c r="H23" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="I23" s="1">
-        <f t="shared" si="1"/>
-        <v>22.5</v>
-      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24">
-        <v>6</v>
-      </c>
+      <c r="F24" s="2"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25">
-        <v>6</v>
-      </c>
-      <c r="H25" s="1">
-        <v>25.95</v>
-      </c>
-      <c r="I25" s="1">
-        <f t="shared" ref="I25" si="2">G25*H25</f>
-        <v>155.69999999999999</v>
-      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F26" s="2"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J17" r:id="rId2"/>
+    <hyperlink ref="J3" r:id="rId3"/>
+    <hyperlink ref="J11"/>
+    <hyperlink ref="J10" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
* Updated architecture schematic to include labels for each device * added Docs folder * Added initial version of architecture document
</commit_message>
<xml_diff>
--- a/platoon/logistics/plattonPartsList.xlsx
+++ b/platoon/logistics/plattonPartsList.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="CART_ITEM" localSheetId="0">Sheet1!$A$5</definedName>
+    <definedName name="CART_ITEM" localSheetId="0">Sheet1!$A$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -241,9 +241,6 @@
     <t>Total / Unit (not including Shipping/Taxes)</t>
   </si>
   <si>
-    <t>Stuff to buy</t>
-  </si>
-  <si>
     <t>On backorder until 4/3
 http://www.newark.com/jsp/search/productdetail.jsp?SKU=43W5302&amp;CMP=KNC-GPLA</t>
   </si>
@@ -257,9 +254,6 @@
     <t>https://www.sparkfun.com/products/7914</t>
   </si>
   <si>
-    <t>Already purchased (includes taxes and shipping)</t>
-  </si>
-  <si>
     <t>DEV-07914</t>
   </si>
   <si>
@@ -281,10 +275,16 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Total for remaining items</t>
-  </si>
-  <si>
     <t>https://www.sparkfun.com/products/709</t>
+  </si>
+  <si>
+    <t>Total for remaining items (shipping/taxes not included)</t>
+  </si>
+  <si>
+    <t>BUY THE STUFF BELOW HERE:</t>
+  </si>
+  <si>
+    <t>Already purchased</t>
   </si>
 </sst>
 </file>
@@ -343,7 +343,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,6 +359,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -473,18 +497,57 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -787,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A2:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,432 +868,413 @@
     <col min="10" max="10" width="119.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="3" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B3" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="10">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4">
-        <v>35</v>
-      </c>
-      <c r="I2" s="4">
-        <f>G2*H2</f>
-        <v>35</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="10">
-        <v>801</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="10"/>
+        <v>33</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="F3" s="11" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="G3" s="10">
         <v>1</v>
       </c>
       <c r="H3" s="4">
-        <v>15.95</v>
+        <v>35</v>
       </c>
       <c r="I3" s="4">
         <f>G3*H3</f>
-        <v>15.95</v>
+        <v>35</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+      <c r="B4" s="10">
+        <v>801</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="10"/>
+        <v>46</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="E4" s="10"/>
       <c r="F4" s="11" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G4" s="10">
         <v>1</v>
       </c>
       <c r="H4" s="4">
-        <v>6.95</v>
+        <v>15.95</v>
       </c>
       <c r="I4" s="4">
         <f>G4*H4</f>
+        <v>15.95</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="10">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
         <v>6.95</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="I5" s="4">
+        <f>G5*H5</f>
+        <v>6.95</v>
+      </c>
+      <c r="J5" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B6" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="14">
-        <v>1</v>
-      </c>
-      <c r="H5" s="16">
-        <v>3.95</v>
-      </c>
-      <c r="I5" s="16">
-        <f>G5*H5</f>
-        <v>3.95</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>8</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="14">
-        <v>22</v>
-      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
       <c r="F6" s="15" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="G6" s="14">
         <v>1</v>
       </c>
       <c r="H6" s="16">
-        <v>20.329999999999998</v>
+        <v>3.95</v>
       </c>
       <c r="I6" s="16">
-        <f t="shared" ref="I6:I17" si="0">G6*H6</f>
-        <v>20.329999999999998</v>
+        <f>G6*H6</f>
+        <v>3.95</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="C7" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
+      <c r="D7" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="14">
+        <v>22</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>40</v>
+      </c>
       <c r="G7" s="14">
         <v>1</v>
       </c>
       <c r="H7" s="16">
+        <v>20.329999999999998</v>
+      </c>
+      <c r="I7" s="16">
+        <f t="shared" ref="I7:I18" si="0">G7*H7</f>
+        <v>20.329999999999998</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="14">
+        <v>1</v>
+      </c>
+      <c r="H8" s="16">
         <v>0</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I8" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J8" s="14" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="10">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4">
-        <v>13.33</v>
-      </c>
-      <c r="I8" s="4">
-        <f t="shared" si="0"/>
-        <v>13.33</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>13.33</v>
+      </c>
       <c r="I9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="10"/>
+        <v>13.33</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>10</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4">
-        <v>25.95</v>
-      </c>
+      <c r="F10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="4"/>
       <c r="I10" s="4">
         <f t="shared" si="0"/>
-        <v>25.95</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>65</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>30</v>
+      <c r="A11" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>58</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="11" t="s">
-        <v>31</v>
-      </c>
+      <c r="F11" s="11"/>
       <c r="G11" s="10">
         <v>1</v>
       </c>
       <c r="H11" s="4">
-        <v>9.99</v>
+        <v>25.95</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="0"/>
-        <v>9.99</v>
+        <v>25.95</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>58</v>
+      </c>
       <c r="E12" s="10"/>
       <c r="F12" s="11" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G12" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H12" s="4">
-        <v>0.51</v>
+        <v>9.99</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="0"/>
-        <v>1.53</v>
+        <v>9.99</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>19</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="12" t="s">
-        <v>23</v>
+      <c r="F13" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="G13" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13" s="4">
-        <v>15.95</v>
+        <v>0.51</v>
       </c>
       <c r="I13" s="4">
         <f t="shared" si="0"/>
-        <v>15.95</v>
-      </c>
-      <c r="J13" s="10"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.53</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G14" s="10">
         <v>1</v>
       </c>
       <c r="H14" s="4">
-        <v>0.95</v>
+        <v>15.95</v>
       </c>
       <c r="I14" s="4">
         <f t="shared" si="0"/>
-        <v>0.95</v>
+        <v>15.95</v>
       </c>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="E15" s="10"/>
       <c r="F15" s="12" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G15" s="10">
-        <v>6</v>
-      </c>
-      <c r="H15" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.95</v>
+      </c>
       <c r="I15" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="10"/>
+        <v>13</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="12"/>
+      <c r="F16" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="G16" s="10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4">
@@ -1241,7 +1285,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -1259,364 +1303,383 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="10">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="21"/>
-    </row>
-    <row r="19" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="24" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="21"/>
+    </row>
+    <row r="20" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26">
-        <f>SUM(I2:I17)</f>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26">
+        <f>SUM(I3:I18)</f>
         <v>149.88</v>
       </c>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" ht="45.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
-      <c r="B20" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="27">
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
+      <c r="B21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="27">
         <v>227.22</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="40">
+        <v>6</v>
+      </c>
+      <c r="H26" s="42">
+        <v>35</v>
+      </c>
+      <c r="I26" s="42">
+        <f t="shared" ref="I26:I32" si="1">G26*H26</f>
+        <v>210</v>
+      </c>
+      <c r="J26" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="40">
+        <v>801</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="40"/>
+      <c r="F27" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="40">
+        <v>6</v>
+      </c>
+      <c r="H27" s="42">
+        <v>15.95</v>
+      </c>
+      <c r="I27" s="42">
+        <f t="shared" si="1"/>
+        <v>95.699999999999989</v>
+      </c>
+      <c r="J27" s="44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="46">
+        <v>6</v>
+      </c>
+      <c r="H28" s="48">
         <v>0</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="10" t="s">
+      <c r="I28" s="48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="46">
+        <v>6</v>
+      </c>
+      <c r="H29" s="48">
+        <v>0</v>
+      </c>
+      <c r="I29" s="48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="46"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="50"/>
+      <c r="F30" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" s="50">
+        <v>36</v>
+      </c>
+      <c r="H30" s="53">
+        <v>0.50760000000000005</v>
+      </c>
+      <c r="I30" s="53">
+        <f t="shared" si="1"/>
+        <v>18.273600000000002</v>
+      </c>
+      <c r="J30" s="54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" s="32">
+        <v>6</v>
+      </c>
+      <c r="H31" s="34">
+        <v>25.95</v>
+      </c>
+      <c r="I31" s="34">
+        <f t="shared" si="1"/>
+        <v>155.69999999999999</v>
+      </c>
+      <c r="J31" s="35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="32"/>
+      <c r="C32" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="32"/>
+      <c r="F32" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="32">
+        <v>6</v>
+      </c>
+      <c r="H32" s="34">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I32" s="34">
+        <f t="shared" si="1"/>
+        <v>59.699999999999996</v>
+      </c>
+      <c r="J32" s="35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="32"/>
+      <c r="F33" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="32">
+        <v>6</v>
+      </c>
+      <c r="H33" s="34">
+        <v>15.95</v>
+      </c>
+      <c r="I33" s="34">
+        <f t="shared" ref="I33:I34" si="2">G33*H33</f>
+        <v>95.699999999999989</v>
+      </c>
+      <c r="J33" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" s="10">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="32"/>
+      <c r="F34" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="G34" s="32">
         <v>6</v>
       </c>
-      <c r="H25" s="4">
-        <v>35</v>
-      </c>
-      <c r="I25" s="4">
-        <f>G25*H25</f>
-        <v>210</v>
-      </c>
-      <c r="J25" s="28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="10">
-        <v>801</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="10">
-        <v>6</v>
-      </c>
-      <c r="H26" s="4">
-        <v>15.95</v>
-      </c>
-      <c r="I26" s="4">
-        <f>G26*H26</f>
-        <v>95.699999999999989</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="10">
-        <v>6</v>
-      </c>
-      <c r="H27" s="4">
-        <v>0</v>
-      </c>
-      <c r="I27" s="4">
-        <f>G27*H27</f>
-        <v>0</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G28" s="10">
-        <v>6</v>
-      </c>
-      <c r="H28" s="4">
-        <v>0</v>
-      </c>
-      <c r="I28" s="4">
-        <f>G28*H28</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="10"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="11" t="s">
+      <c r="H34" s="34">
+        <v>0.95</v>
+      </c>
+      <c r="I34" s="34">
+        <f t="shared" si="2"/>
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="J34" s="35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="I35" s="30">
+        <f>SUM(I26:I34)</f>
+        <v>640.77359999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="F38" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="10">
-        <v>36</v>
-      </c>
-      <c r="H29" s="4">
-        <v>0.50760000000000005</v>
-      </c>
-      <c r="I29" s="4">
-        <f>G29*H29</f>
-        <v>18.273600000000002</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G30" s="10">
-        <v>6</v>
-      </c>
-      <c r="H30" s="4">
-        <v>25.95</v>
-      </c>
-      <c r="I30" s="4">
-        <f>G30*H30</f>
-        <v>155.69999999999999</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" s="10">
-        <v>6</v>
-      </c>
-      <c r="H31" s="4">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="I31" s="4">
-        <f>G31*H31</f>
-        <v>59.699999999999996</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="10">
-        <v>6</v>
-      </c>
-      <c r="H32" s="4">
-        <v>15.95</v>
-      </c>
-      <c r="I32" s="4">
-        <f t="shared" ref="I32:I33" si="1">G32*H32</f>
-        <v>95.699999999999989</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G33" s="10">
-        <v>6</v>
-      </c>
-      <c r="H33" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="I33" s="4">
-        <f t="shared" si="1"/>
-        <v>5.6999999999999993</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="I34" s="33">
-        <f>SUM(I25:I33)</f>
-        <v>640.77359999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="F37" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="23">
-        <f>SUM(C20,I34)</f>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="23">
+        <f>SUM(C21,I35)</f>
         <v>867.99360000000001</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J12" display="http://www.digikey.com/product-detail/en/TIP120/TIP120-ND/1052441?adpos=1t2&amp;WT.term=tip120&amp;WT.mc_id=Fairchild+Semiconductor&amp;WT.medium=cpc&amp;WT.campaign=Fairchild+Semiconductor&amp;WT.content=text&amp;WT.srch=1&amp;type=Phrase&amp;WT.source=google&amp;cshift_ck=C7AE7C92-6598-4F"/>
-    <hyperlink ref="J11" r:id="rId3"/>
-    <hyperlink ref="J10" r:id="rId4"/>
-    <hyperlink ref="J25" r:id="rId5" display="http://www.newark.com/jsp/search/productdetail.jsp?SKU=43W5302&amp;CMP=KNC-GPLA"/>
-    <hyperlink ref="J26" r:id="rId6"/>
-    <hyperlink ref="J30" r:id="rId7"/>
-    <hyperlink ref="J29" r:id="rId8"/>
-    <hyperlink ref="J32" r:id="rId9"/>
-    <hyperlink ref="J33" r:id="rId10"/>
-    <hyperlink ref="J31" r:id="rId11"/>
+    <hyperlink ref="J3" r:id="rId1"/>
+    <hyperlink ref="J4" r:id="rId2"/>
+    <hyperlink ref="J13" display="http://www.digikey.com/product-detail/en/TIP120/TIP120-ND/1052441?adpos=1t2&amp;WT.term=tip120&amp;WT.mc_id=Fairchild+Semiconductor&amp;WT.medium=cpc&amp;WT.campaign=Fairchild+Semiconductor&amp;WT.content=text&amp;WT.srch=1&amp;type=Phrase&amp;WT.source=google&amp;cshift_ck=C7AE7C92-6598-4F"/>
+    <hyperlink ref="J12" r:id="rId3"/>
+    <hyperlink ref="J11" r:id="rId4"/>
+    <hyperlink ref="J26" r:id="rId5" display="http://www.newark.com/jsp/search/productdetail.jsp?SKU=43W5302&amp;CMP=KNC-GPLA"/>
+    <hyperlink ref="J27" r:id="rId6"/>
+    <hyperlink ref="J31" r:id="rId7"/>
+    <hyperlink ref="J30" r:id="rId8"/>
+    <hyperlink ref="J33" r:id="rId9"/>
+    <hyperlink ref="J34" r:id="rId10"/>
+    <hyperlink ref="J32" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>

</xml_diff>

<commit_message>
* Adding Firmatoon sketch.  This is a modified version of the standard Firmata sketch with the LCD modifications in it * Updates to Architecture schematic.  Wiring on LCD was off. Reference LCD.fzz for standard * Created arduino folder for all arduino sketches
</commit_message>
<xml_diff>
--- a/platoon/logistics/plattonPartsList.xlsx
+++ b/platoon/logistics/plattonPartsList.xlsx
@@ -327,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,19 +354,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,7 +426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -480,24 +474,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -509,6 +485,18 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -815,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,7 +1337,7 @@
     </row>
     <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="35" t="s">
         <v>79</v>
       </c>
       <c r="C21" s="12">
@@ -1371,271 +1359,271 @@
       <c r="I24" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="27">
+      <c r="G26" s="37">
         <v>6</v>
       </c>
-      <c r="H26" s="28">
+      <c r="H26" s="39">
         <v>35</v>
       </c>
-      <c r="I26" s="28">
+      <c r="I26" s="39">
         <f t="shared" ref="I26:I32" si="2">G26*H26</f>
         <v>210</v>
       </c>
-      <c r="J26" s="29" t="s">
+      <c r="J26" s="41" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="37">
         <v>801</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="27"/>
-      <c r="F27" s="26" t="s">
+      <c r="E27" s="37"/>
+      <c r="F27" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="37">
         <v>6</v>
       </c>
-      <c r="H27" s="28">
+      <c r="H27" s="39">
         <v>15.95</v>
       </c>
-      <c r="I27" s="28">
+      <c r="I27" s="39">
         <f t="shared" si="2"/>
         <v>95.699999999999989</v>
       </c>
-      <c r="J27" s="30" t="s">
+      <c r="J27" s="40" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="31" t="s">
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="32">
+      <c r="G28" s="27">
         <v>6</v>
       </c>
-      <c r="H28" s="33">
+      <c r="H28" s="28">
         <v>0</v>
       </c>
-      <c r="I28" s="33">
+      <c r="I28" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J28" s="31" t="s">
+      <c r="J28" s="26" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32" t="s">
+      <c r="B29" s="27"/>
+      <c r="C29" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="31" t="s">
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="G29" s="32">
+      <c r="G29" s="27">
         <v>6</v>
       </c>
-      <c r="H29" s="33">
+      <c r="H29" s="28">
         <v>0</v>
       </c>
-      <c r="I29" s="33">
+      <c r="I29" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J29" s="32"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35" t="s">
+      <c r="B30" s="37"/>
+      <c r="C30" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="36" t="s">
+      <c r="D30" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="35"/>
-      <c r="F30" s="34" t="s">
+      <c r="E30" s="37"/>
+      <c r="F30" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="G30" s="35">
+      <c r="G30" s="37">
         <v>36</v>
       </c>
-      <c r="H30" s="37">
+      <c r="H30" s="39">
         <v>0.50760000000000005</v>
       </c>
-      <c r="I30" s="37">
+      <c r="I30" s="39">
         <f t="shared" si="2"/>
         <v>18.273600000000002</v>
       </c>
-      <c r="J30" s="38" t="s">
+      <c r="J30" s="40" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D31" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="40"/>
-      <c r="F31" s="39" t="s">
+      <c r="E31" s="30"/>
+      <c r="F31" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="40">
+      <c r="G31" s="30">
         <v>6</v>
       </c>
-      <c r="H31" s="42">
+      <c r="H31" s="32">
         <v>25.95</v>
       </c>
-      <c r="I31" s="42">
+      <c r="I31" s="32">
         <f t="shared" si="2"/>
         <v>155.69999999999999</v>
       </c>
-      <c r="J31" s="43" t="s">
+      <c r="J31" s="33" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="44" t="s">
+      <c r="B32" s="30"/>
+      <c r="C32" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="41" t="s">
+      <c r="D32" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="40"/>
-      <c r="F32" s="39" t="s">
+      <c r="E32" s="30"/>
+      <c r="F32" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G32" s="40">
+      <c r="G32" s="30">
         <v>6</v>
       </c>
-      <c r="H32" s="42">
+      <c r="H32" s="32">
         <v>9.9499999999999993</v>
       </c>
-      <c r="I32" s="42">
+      <c r="I32" s="32">
         <f t="shared" si="2"/>
         <v>59.699999999999996</v>
       </c>
-      <c r="J32" s="43" t="s">
+      <c r="J32" s="33" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="40" t="s">
+      <c r="D33" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="39" t="s">
+      <c r="E33" s="30"/>
+      <c r="F33" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="40">
+      <c r="G33" s="30">
         <v>6</v>
       </c>
-      <c r="H33" s="42">
+      <c r="H33" s="32">
         <v>15.95</v>
       </c>
-      <c r="I33" s="42">
+      <c r="I33" s="32">
         <f t="shared" ref="I33:I34" si="3">G33*H33</f>
         <v>95.699999999999989</v>
       </c>
-      <c r="J33" s="43" t="s">
+      <c r="J33" s="33" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="40"/>
-      <c r="F34" s="39" t="s">
+      <c r="E34" s="30"/>
+      <c r="F34" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="G34" s="40">
+      <c r="G34" s="30">
         <v>6</v>
       </c>
-      <c r="H34" s="42">
+      <c r="H34" s="32">
         <v>0.95</v>
       </c>
-      <c r="I34" s="42">
+      <c r="I34" s="32">
         <f t="shared" si="3"/>
         <v>5.6999999999999993</v>
       </c>
-      <c r="J34" s="43" t="s">
+      <c r="J34" s="33" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated parts list and small changes to OSC scripts
</commit_message>
<xml_diff>
--- a/platoon/logistics/plattonPartsList.xlsx
+++ b/platoon/logistics/plattonPartsList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="83">
   <si>
     <t>Raspberry Pi</t>
   </si>
@@ -261,6 +261,15 @@
   </si>
   <si>
     <t>Already purchased</t>
+  </si>
+  <si>
+    <t>Orders total</t>
+  </si>
+  <si>
+    <t>SparkFun</t>
+  </si>
+  <si>
+    <t>Newegg</t>
   </si>
 </sst>
 </file>
@@ -426,7 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -474,16 +483,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -499,6 +498,8 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -801,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J38"/>
+  <dimension ref="A2:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1338,7 @@
     </row>
     <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="29" t="s">
         <v>79</v>
       </c>
       <c r="C21" s="12">
@@ -1359,66 +1360,66 @@
       <c r="I24" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="E26" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="36" t="s">
+      <c r="F26" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="37">
+      <c r="G26" s="31">
         <v>6</v>
       </c>
-      <c r="H26" s="39">
+      <c r="H26" s="33">
         <v>35</v>
       </c>
-      <c r="I26" s="39">
+      <c r="I26" s="33">
         <f t="shared" ref="I26:I32" si="2">G26*H26</f>
         <v>210</v>
       </c>
-      <c r="J26" s="41" t="s">
+      <c r="J26" s="35" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="37">
+      <c r="B27" s="31">
         <v>801</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="37"/>
-      <c r="F27" s="36" t="s">
+      <c r="E27" s="31"/>
+      <c r="F27" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="37">
+      <c r="G27" s="31">
         <v>6</v>
       </c>
-      <c r="H27" s="39">
+      <c r="H27" s="33">
         <v>15.95</v>
       </c>
-      <c r="I27" s="39">
+      <c r="I27" s="33">
         <f t="shared" si="2"/>
         <v>95.699999999999989</v>
       </c>
-      <c r="J27" s="40" t="s">
+      <c r="J27" s="34" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1477,153 +1478,153 @@
       <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37" t="s">
+      <c r="B30" s="31"/>
+      <c r="C30" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="38" t="s">
+      <c r="D30" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="37"/>
-      <c r="F30" s="36" t="s">
+      <c r="E30" s="31"/>
+      <c r="F30" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="G30" s="37">
+      <c r="G30" s="31">
         <v>36</v>
       </c>
-      <c r="H30" s="39">
+      <c r="H30" s="33">
         <v>0.50760000000000005</v>
       </c>
-      <c r="I30" s="39">
+      <c r="I30" s="33">
         <f t="shared" si="2"/>
         <v>18.273600000000002</v>
       </c>
-      <c r="J30" s="40" t="s">
+      <c r="J30" s="34" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="29" t="s">
+      <c r="E31" s="31"/>
+      <c r="F31" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="30">
+      <c r="G31" s="31">
         <v>6</v>
       </c>
-      <c r="H31" s="32">
+      <c r="H31" s="33">
         <v>25.95</v>
       </c>
-      <c r="I31" s="32">
+      <c r="I31" s="33">
         <f t="shared" si="2"/>
         <v>155.69999999999999</v>
       </c>
-      <c r="J31" s="33" t="s">
+      <c r="J31" s="34" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="34" t="s">
+      <c r="B32" s="31"/>
+      <c r="C32" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="29" t="s">
+      <c r="E32" s="31"/>
+      <c r="F32" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="G32" s="30">
+      <c r="G32" s="31">
         <v>6</v>
       </c>
-      <c r="H32" s="32">
+      <c r="H32" s="33">
         <v>9.9499999999999993</v>
       </c>
-      <c r="I32" s="32">
+      <c r="I32" s="33">
         <f t="shared" si="2"/>
         <v>59.699999999999996</v>
       </c>
-      <c r="J32" s="33" t="s">
+      <c r="J32" s="34" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="29" t="s">
+      <c r="E33" s="31"/>
+      <c r="F33" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="30">
+      <c r="G33" s="31">
         <v>6</v>
       </c>
-      <c r="H33" s="32">
+      <c r="H33" s="33">
         <v>15.95</v>
       </c>
-      <c r="I33" s="32">
+      <c r="I33" s="33">
         <f t="shared" ref="I33:I34" si="3">G33*H33</f>
         <v>95.699999999999989</v>
       </c>
-      <c r="J33" s="33" t="s">
+      <c r="J33" s="34" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="30"/>
-      <c r="F34" s="29" t="s">
+      <c r="E34" s="31"/>
+      <c r="F34" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G34" s="30">
+      <c r="G34" s="31">
         <v>6</v>
       </c>
-      <c r="H34" s="32">
+      <c r="H34" s="33">
         <v>0.95</v>
       </c>
-      <c r="I34" s="32">
+      <c r="I34" s="33">
         <f t="shared" si="3"/>
         <v>5.6999999999999993</v>
       </c>
-      <c r="J34" s="33" t="s">
+      <c r="J34" s="34" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1647,6 +1648,47 @@
       <c r="I38" s="8">
         <f>SUM(C21,I35)</f>
         <v>867.99360000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41">
+        <v>28.94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42">
+        <v>332.03</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43">
+        <f>25.48+64.44+159.3</f>
+        <v>249.22000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="37">
+        <f>SUM(B40:B43)</f>
+        <v>610.19000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>